<commit_message>
trying to get sink filler to work
</commit_message>
<xml_diff>
--- a/last_chance_experiments/GSDs/LC1_grain_size_dist.xlsx
+++ b/last_chance_experiments/GSDs/LC1_grain_size_dist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sam\MultiGrain\working_folder\GSDs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sam\MultiGrain\last_chance_experiments\GSDs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B02631F-B97C-4898-9141-F781B63D9133}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0835CB84-A111-4B7D-9555-57E0DAADAD50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2592" yWindow="6096" windowWidth="7500" windowHeight="6000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GSD" sheetId="1" r:id="rId1"/>
@@ -371,12 +371,12 @@
   <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.21875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
@@ -744,7 +744,7 @@
         <v>0.41152263374485598</v>
       </c>
       <c r="D26">
-        <v>27.945205479452056</v>
+        <v>28.082191780821919</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>